<commit_message>
performing NLP subdomain analysis
</commit_message>
<xml_diff>
--- a/S18_NLP_With_Results_FOR_ANALYSIS.xlsx
+++ b/S18_NLP_With_Results_FOR_ANALYSIS.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claytoncohn/Dropbox/MMLTE/MMLTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2DC5F57B-78CC-F945-891C-3193FF355F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97905BD-8875-CD45-9779-6C67C3925319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S18_NLP_With_Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">S18_NLP_With_Results!$A$1:$Q$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">S18_NLP_With_Results!$A$1:$S$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="280">
   <si>
     <t>UUID</t>
   </si>
@@ -875,11 +875,116 @@
     <t>"We found that the semantics and speaker information in the linguistic modality, the pitch variation in the audio modality, and the facial muscle movements in the video modality are the most significant unimodal indicators of impasse."
 "We found that the semantics and speaker information in the linguistic modality, the pitch variation in the audio modality, and the facial muscle movements in the video modality are the most significant unimodal indicators of impasse. We also trained several multimodal models and found that combining indicators from these three modalities provided the best impasse detection performance."</t>
   </si>
+  <si>
+    <t>Challenges</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>ASR issues</t>
+  </si>
+  <si>
+    <t>CPS, PELARS</t>
+  </si>
+  <si>
+    <t>CPS, PELARS, Audio Level feature</t>
+  </si>
+  <si>
+    <t>ASD agent, limitation that utterance content is not used.</t>
+  </si>
+  <si>
+    <t>Collaborative, in-person engineering tasks with real materials.</t>
+  </si>
+  <si>
+    <t>Virtual debate coach. Prosodics only.</t>
+  </si>
+  <si>
+    <t>Virtual debate coach.</t>
+  </si>
+  <si>
+    <t>A fully automatic system that is able to understand natu-
+ral arguments in a debate accurately enough to achieve human-like
+performance has not been yet achieved due to certain limitations in
+sensor tracking, speech recognition, and natural language process-
+ing technologies. Also since a data-oriented approach for modelling
+of many debate phenomena has been deployed, the currently avail-
+able quantity and quality of multimodal data are insufficient fortraining statistical machine learning algorithms.
+Hardware issues, data issues.</t>
+  </si>
+  <si>
+    <t>Collaboration, CSCL</t>
+  </si>
+  <si>
+    <t>Challenges w/ mobile mixed-reality learning.</t>
+  </si>
+  <si>
+    <t>Mobile Mixed Reality sim learning.</t>
+  </si>
+  <si>
+    <t>Math, collaboration.</t>
+  </si>
+  <si>
+    <t>ITS Agent</t>
+  </si>
+  <si>
+    <t>Collaborative.</t>
+  </si>
+  <si>
+    <t>In practice, however, the increased complexity resulting from the additional collection of multimodal data presents
+unique challenges. Data from different sources are often difficult to integrate. Making sense of all the richness that exists in
+multimodal data can be highly time-consuming. Imagine trying to understand the detailed sequence of events a student
+exhibits as he/she engages in productive struggle with a difficult concept and the social interactions surrounding this effort.
+To fully understand the events that unfold even in this small segment of a student’s educational experience, a researcher may
+need to watch screen video data and listen to the audio dialogue several times and enter behavioural codes into a separate
+document. Having to do this for every problem and concept a student experiences over the course of even one class period of
+learning technology use would be vastly taxing on human time and effort.
+Temporality
+Complexity</t>
+  </si>
+  <si>
+    <t>In practice, however, the increased complexity of data resulting from
+adding new, multimodal data streams from different sources can create
+many challenges. These data are often collected at different grain sizes,
+which are difficult to integrate. Making sense of data at many levels of
+analysis, including the most detailed levels, is highly time‐consuming.
+Imagine trying to understand the detailed sequence of events a student
+exhibits as he or she engages in productive struggle with a difficult
+concept and the social interactions surrounding this struggle. To fully
+understand the events that unfold even in this small segment of a
+student's educational experience, a researcher may need to watch screen
+video data, listen to the audio dialogue several times, and enter
+behavioural codes into a separate document. Having to do this for every
+problem and concept students experience over the course of even one
+class period of learning technology use would be vastly taxing on human
+time and effort. Yet this level of detailed analysis provides interesting and
+temporally rich insights (Worsley, 2014), in contrast to purely quantitative
+models based solely on coarse‐level “correctness” coding.
+One of the biggest challenges in multimodal learning analytics is
+that the large volume of rich, multimodal data collected requires signif-
+icant human time and effort to make sense of.
+Complexity</t>
+  </si>
+  <si>
+    <t>for complexity challenge: "The eye-tracking glasses sampled at a rate of 50
+Hz, thus generating roughly 90,000 data points per person during the 30-minute session."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indeed, the understanding of specific problems and phenomena that arise in the implementation of educational innovations in authentic settings (also known as ‘orchestration’) is considered one of the foremost challenges in the
+field of TEL (Fischer et al. 2014; Roschelle et al. 2013).
+From the audio data, 6405 features were extracted using the openSMILE audio
+processing toolkit (http://audeering.com/technology/opensmile/). The features
+extracted included both high-level constructs (e.g., emotion detection
+predictions) as well as low-level features of the spectrum, energy, etc. of each
+episode (commonly used in audio data mining and machine learning challenges).
+Complexity with so many features.
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1728,11 +1833,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="77.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1757,7 +1863,7 @@
     <col min="18" max="16384" width="77.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1809,8 +1915,14 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>261</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1118315889</v>
       </c>
@@ -1862,8 +1974,14 @@
       <c r="Q2" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="R2" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>3339002981</v>
       </c>
@@ -1915,8 +2033,11 @@
       <c r="Q3" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="S3" s="1" t="s">
+        <v>264</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" ht="221" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="221" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3093310941</v>
       </c>
@@ -1968,8 +2089,11 @@
       <c r="Q4" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="S4" s="1" t="s">
+        <v>265</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" ht="306" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="306" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3095923626</v>
       </c>
@@ -2021,8 +2145,11 @@
       <c r="Q5" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="S5" s="1" t="s">
+        <v>266</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" ht="204" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>85990093</v>
       </c>
@@ -2074,8 +2201,11 @@
       <c r="Q6" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="S6" s="1" t="s">
+        <v>267</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="204" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="204" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>957160695</v>
       </c>
@@ -2127,8 +2257,14 @@
       <c r="Q7" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="R7" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" ht="356" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="356" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1637690235</v>
       </c>
@@ -2180,8 +2316,11 @@
       <c r="Q8" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="S8" s="1" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2181637610</v>
       </c>
@@ -2233,8 +2372,14 @@
       <c r="Q9" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="R9" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>270</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" ht="187" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="187" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>3146393211</v>
       </c>
@@ -2286,8 +2431,14 @@
       <c r="Q10" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="R10" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>272</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" ht="153" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="221" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>3135645357</v>
       </c>
@@ -2339,8 +2490,14 @@
       <c r="Q11" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="R11" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>273</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" ht="221" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="306" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>3783339081</v>
       </c>
@@ -2392,8 +2549,14 @@
       <c r="Q12" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="R12" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
-    <row r="13" spans="1:17" ht="238" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="388" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>3796180663</v>
       </c>
@@ -2445,8 +2608,14 @@
       <c r="Q13" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="R13" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="14" spans="1:17" ht="221" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="221" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2345021698</v>
       </c>
@@ -2499,7 +2668,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="238" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="238" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2497456347</v>
       </c>
@@ -2552,7 +2721,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="170" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="170" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>4019205162</v>
       </c>
@@ -3666,7 +3835,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q36"/>
+  <autoFilter ref="A1:S1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished NLP subdomain feature extraction and notes. will finish analysis tomorrow for results, challenges, and SOTA
</commit_message>
<xml_diff>
--- a/S18_NLP_With_Results_FOR_ANALYSIS.xlsx
+++ b/S18_NLP_With_Results_FOR_ANALYSIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claytoncohn/Dropbox/MMLTE/MMLTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13359BC-2574-3847-A72F-04CBD44B5A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8474299-2AAA-0D45-BB2B-1E837A79E66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="353">
   <si>
     <t>UUID</t>
   </si>
@@ -779,11 +779,6 @@
     <t>IJCSCL</t>
   </si>
   <si>
-    <t>"Our combined multi-modal learning analytics and interaction analysis methodology enabled us to identify two multi-modal profles of learners who have learning gains and one multi-modal profle of learners who do not have learning gains."
-"Using this approach, we are able to build the multimodal behavioral profles for each group of learners."
-"Our combined multi-modal learning analytics and interaction analysis methodology enabled us to identify two multi-modal profles of learners who have learning gains and one multi-modal profle of learners who do not have learning gains."</t>
-  </si>
-  <si>
     <t>once more with feeling: emotions in multimodal learning analytics</t>
   </si>
   <si>
@@ -870,10 +865,6 @@
   </si>
   <si>
     <t>TRANS,PROS,SPECT,GAZE,POSE</t>
-  </si>
-  <si>
-    <t>"We found that the semantics and speaker information in the linguistic modality, the pitch variation in the audio modality, and the facial muscle movements in the video modality are the most significant unimodal indicators of impasse."
-"We found that the semantics and speaker information in the linguistic modality, the pitch variation in the audio modality, and the facial muscle movements in the video modality are the most significant unimodal indicators of impasse. We also trained several multimodal models and found that combining indicators from these three modalities provided the best impasse detection performance."</t>
   </si>
   <si>
     <t>Challenges</t>
@@ -1195,6 +1186,151 @@
   <si>
     <t>Text-input difficult for younger students who couldn't yet type.
 Unreliable ASR. We believe that this is due to poor quality acoustic models for adolescents and because many of our participants spoke other languages at home.</t>
+  </si>
+  <si>
+    <t>MMLA to Explore Collaboration in a Sustainability Co-located Tabletop Game. leveraging MMLA to explore collaboration indicators in a multiplayer, co-located SG for education in sustainable development.</t>
+  </si>
+  <si>
+    <t>STATS: Variables originating from the different sources were examined with descriptive statistics. Perceived quality of
+collaboration was correlated with other variables using Pearson correlations. Teams were then categorised
+according to turn score quartiles, which was then used to analyse the relationship between game performance
+and collaboration behaviours using one-way ANOVA.</t>
+  </si>
+  <si>
+    <t>Collaborative. identifying multi-modal
+behavioral profles of collaborative learning in constructivist
+activities. we describe a combined multi-modal learning analytics and interaction analysis method that uses video, audio and log data to identify multi-modal
+collaborative learning behavioral profles of 32 dyads as they work on an open-ended
+task around interactive tabletops with a robot mediator.</t>
+  </si>
+  <si>
+    <t>"Our combined multi-modal learning analytics and interaction analysis methodology enabled us to identify two multi-modal profles of learners who have learning gains and one multi-modal profle of learners who do not have learning gains."
+"Using this approach, we are able to build the multimodal behavioral profles for each group of learners."
+"Our combined multi-modal learning analytics and interaction analysis methodology enabled us to identify two multi-modal profles of learners who have learning gains and one multi-modal profle of learners who do not have learning gains."
+These profles, which we name Expressive Explorers, Calm Tinkerers, and Silent Wanderers, confrm previous collaborative learning fndings. In particular, the amount of speech interaction and the overlap of speech between a pair of learners are behavior patterns that strongly distinguish between learning and non-learning pairs.</t>
+  </si>
+  <si>
+    <t>STATS: p-values for the Kruskal-Wallis analysis on each pair with signifcance level of 0.05
+QUAL: interaction analysis
+CLUST: cluster learning and performance measures and also multi-modal behaviors
+CLS: SVM and Random Forests</t>
+  </si>
+  <si>
+    <t>The data
+driven clusters are imbalanced, meaning that with our pipeline, the non-learning cluster
+that emerges has fewer teams. This may be one of the reasons why the gainer profles
+are clearer compared to the Silent Wanderers profle (overall challenge)</t>
+  </si>
+  <si>
+    <t>Emotions in MMLA. We use NLP and machine learning
+techniques to automatically extract information about students’ motivational states while engaging in the construction of explanations and investigate how this informa-
+tion can help more accurately predict students’ learning over the course of a 10-week energy unit.</t>
+  </si>
+  <si>
+    <t>extensive preprocessing of the data and the results need to be
+interpreted with care and caution (overall challenge)
+data in a real learning environment
+is noisy, not structured and context dependent.
+we struggled with
+identifying the audio segments which contained students’ interaction.
+speaker diarization, the task of identifying who is speaking and when, has
+caught the attention of researchers and there are several methods which perform
+quite well.
+state-of-the-art diarization system does not perform well on
+real child-speech interactions,
+difficulties segmenting the audio files in order to obtain the students-only utterances
+we decided to split the audio manually, which
+was time consuming and, therefore, led to a lower number of students considered in
+the applied example.
+Obtaining and labelling data is indeed a costly process especially in the context
+of education (overall challenge)
+data is limited, which represents one of the major
+challenges for building robust and reliable multimodal models. (oveall challenge)
+training a
+model on a reduced dataset introduces a bias to the model, affecting the validity
+of the model’s predictions when the data inputs come from a different distribution
+than the training set. (oveall challenge)
+lack of representative data in open datasets (i.e., few focusing on children/education) (overall challenge)</t>
+  </si>
+  <si>
+    <t>CLS: OpenVokaturi SDK emotion detection
+REG: Regression results for valence/discrete emotions. Dependent variable students’ knowledge-in-use about
+energy after the unit. we used regression models to further investigate how valence could help us
+to better understand students’ performance on the energy test after the unit.
+STATS: correlations between valence, students’
+energy knowledge-in-use after the unit, and their mastery goal orientation, w/ p-value</t>
+  </si>
+  <si>
+    <t>Collab. We present a MMLA platform to support
+collaboration assessment based on the capture and classification of non-verbal communication in-
+teractions.</t>
+  </si>
+  <si>
+    <t>QUAL: Case study. we decided to compare two different teamwork activities, with
+high contrast between collaborative and non-collaborative work. Field notes allowed us to describe the flow of interaction of
+the subjects and observations about the six collaboration constructs of the framework</t>
+  </si>
+  <si>
+    <t>Finally, the design and sample size of the focus group do not allow us to generalize the
+results. (overall challenge)</t>
+  </si>
+  <si>
+    <t>Recurrence Quantification Analysis (RQA) to quantify the
+microgenesis of stable new patterns in hand movement and gaze.</t>
+  </si>
+  <si>
+    <t>PATT: Recurrence Quantification Analysis (RQA)
+QUAL: To contextualize results within the student’s
+specific learning trajectory, we began with a qualitative analysis of the audio-video
+recording.
+STATS: We also calculated the correlation between each hand’s y-location and
+y-axis gaze position in each task stage as an initial reflection of the relationship
+between these two modalities.</t>
+  </si>
+  <si>
+    <t>Collab. A multimodal analysis of pair work engagement episodes:
+Implications for EMI lecturer training.</t>
+  </si>
+  <si>
+    <t>Data scarcity: The limited number of pair work EEs does not allow us to make any strong claims in terms of
+the framework’s reliability. (overall challenge)</t>
+  </si>
+  <si>
+    <t>QUAL: In the first part, the 12 micro-teaching sessions were carefully watched to identify the pair work EEs (See Table 1). Then, the
+selected EEs were transcribed and examined to determine the moves and pedagogical functions the lecturers performed. In the second part, the microanalysis, we followed a SF-MDA (O’Halloran, 2004) approach to describe how these pedagogical
+functions were constructed multimodally.</t>
+  </si>
+  <si>
+    <t>Collab. This paper inves-
+tigates multimodal detection of impasse by analyzing 46 middle
+school learners’ collaborative dialogue—including speech and facial
+behaviors—during a coding task.</t>
+  </si>
+  <si>
+    <t>CLS: (Speaker-aware) Fine-tuned BERT for impasse classification (and regular fine-tuned BERT), TF-IDF, Word2Vec. Also used SVM, MLP to identify predictive unimodal features.</t>
+  </si>
+  <si>
+    <t>our corpus size was relatively small.
+The recordings were collected from just 46 middle school learners; (overall challenge)</t>
+  </si>
+  <si>
+    <t>"We found that the semantics and speaker information in the linguistic modality, the pitch variation in the audio modality, and the facial muscle movements in the video modality are the most significant unimodal indicators of impasse."
+"We found that the semantics and speaker information in the linguistic modality, the pitch variation in the audio modality, and the facial muscle movements in the video modality are the most significant unimodal indicators of impasse. We also trained several multimodal models and found that combining indicators from these three modalities provided the best impasse detection performance."
+The results showed that Linguistic + Audio + Video (F1 Score
+= 0.65) yielded the best impasse detection performance, and Audio
++ Video (F1 Score = 0.39) performed the worst. There are several
+important implications behind these results. First, all of our multi-
+modal models outperformed their unimodal models (e.g., the Audio
++ Video model outperformed unimodal Audio / Video models, the
+Linguistic + Audio model outperformed unimodal Linguistic / Au-
+dio models), which indicated that combining modalities improves
+impasse detection performance. Second, the close performance from
+the Linguistic + Video model and the Linguistic + Audio + Video
+model suggested that adding acoustic-prosodic features to the Lin-
+guistic + Video model did not make a substantial difference. As
+we discussed in section 6.1.2, the significant rise in pitch when the
+second learner started talking was more correlated with impasse
+moments when learners expressed disagreement;</t>
   </si>
 </sst>
 </file>
@@ -2052,9 +2188,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="77.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2133,13 +2269,13 @@
         <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="119" x14ac:dyDescent="0.2">
@@ -2195,13 +2331,13 @@
         <v>31</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="136" x14ac:dyDescent="0.2">
@@ -2257,10 +2393,10 @@
         <v>38</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="221" x14ac:dyDescent="0.2">
@@ -2316,10 +2452,10 @@
         <v>51</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="306" x14ac:dyDescent="0.2">
@@ -2375,10 +2511,10 @@
         <v>60</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="204" x14ac:dyDescent="0.2">
@@ -2434,13 +2570,13 @@
         <v>68</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="204" x14ac:dyDescent="0.2">
@@ -2496,13 +2632,13 @@
         <v>73</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="356" x14ac:dyDescent="0.2">
@@ -2558,10 +2694,10 @@
         <v>80</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
@@ -2617,13 +2753,13 @@
         <v>88</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="187" x14ac:dyDescent="0.2">
@@ -2679,13 +2815,13 @@
         <v>95</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="221" x14ac:dyDescent="0.2">
@@ -2741,13 +2877,13 @@
         <v>103</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="306" x14ac:dyDescent="0.2">
@@ -2803,13 +2939,13 @@
         <v>110</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="388" x14ac:dyDescent="0.2">
@@ -2865,13 +3001,13 @@
         <v>117</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="221" x14ac:dyDescent="0.2">
@@ -2927,10 +3063,10 @@
         <v>124</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="238" x14ac:dyDescent="0.2">
@@ -2986,13 +3122,13 @@
         <v>132</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="170" x14ac:dyDescent="0.2">
@@ -3048,10 +3184,10 @@
         <v>140</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="204" x14ac:dyDescent="0.2">
@@ -3107,10 +3243,10 @@
         <v>148</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="119" x14ac:dyDescent="0.2">
@@ -3166,13 +3302,13 @@
         <v>154</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="204" x14ac:dyDescent="0.2">
@@ -3228,10 +3364,10 @@
         <v>160</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="289" x14ac:dyDescent="0.2">
@@ -3287,10 +3423,10 @@
         <v>166</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
@@ -3346,10 +3482,10 @@
         <v>172</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="102" x14ac:dyDescent="0.2">
@@ -3405,13 +3541,13 @@
         <v>179</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="153" x14ac:dyDescent="0.2">
@@ -3467,13 +3603,13 @@
         <v>184</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
@@ -3529,10 +3665,10 @@
         <v>190</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="119" x14ac:dyDescent="0.2">
@@ -3588,13 +3724,13 @@
         <v>195</v>
       </c>
       <c r="R25" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="S25" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="S25" s="1" t="s">
-        <v>322</v>
-      </c>
       <c r="T25" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="255" x14ac:dyDescent="0.2">
@@ -3650,13 +3786,13 @@
         <v>201</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="136" x14ac:dyDescent="0.2">
@@ -3712,10 +3848,10 @@
         <v>206</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="153" x14ac:dyDescent="0.2">
@@ -3771,13 +3907,13 @@
         <v>213</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="221" x14ac:dyDescent="0.2">
@@ -3833,13 +3969,13 @@
         <v>218</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="T29" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="388" x14ac:dyDescent="0.2">
@@ -3894,8 +4030,14 @@
       <c r="Q30" s="1" t="s">
         <v>224</v>
       </c>
+      <c r="S30" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>332</v>
+      </c>
     </row>
-    <row r="31" spans="1:20" ht="170" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="255" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2273914836</v>
       </c>
@@ -3945,18 +4087,27 @@
         <v>30</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>231</v>
+        <v>335</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>334</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="153" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>32184286</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="D32" s="1">
         <v>2022</v>
@@ -3965,19 +4116,19 @@
         <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>86</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>25</v>
@@ -3998,15 +4149,24 @@
         <v>116</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>338</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="238" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" ht="238" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2609260641</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>119</v>
@@ -4018,10 +4178,10 @@
         <v>19</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>145</v>
@@ -4030,7 +4190,7 @@
         <v>86</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>25</v>
@@ -4045,24 +4205,33 @@
         <v>59</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>341</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="238" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" ht="238" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>1345598079</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="D34" s="1">
         <v>2022</v>
@@ -4071,19 +4240,19 @@
         <v>19</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>86</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>37</v>
@@ -4104,18 +4273,24 @@
         <v>50</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>344</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="187" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" ht="187" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2155422499</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="D35" s="1">
         <v>2022</v>
@@ -4127,7 +4302,7 @@
         <v>203</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>145</v>
@@ -4136,7 +4311,7 @@
         <v>86</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>25</v>
@@ -4157,18 +4332,27 @@
         <v>50</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>346</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="153" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>3754172825</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="D36" s="1">
         <v>2022</v>
@@ -4180,7 +4364,7 @@
         <v>63</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>35</v>
@@ -4210,7 +4394,16 @@
         <v>30</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>259</v>
+        <v>352</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished NLP subdomain analysis
</commit_message>
<xml_diff>
--- a/S18_NLP_With_Results_FOR_ANALYSIS.xlsx
+++ b/S18_NLP_With_Results_FOR_ANALYSIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claytoncohn/Dropbox/MMLTE/MMLTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8474299-2AAA-0D45-BB2B-1E837A79E66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67FD39E-176F-0E42-BEFD-3DEA30B80A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,10 +140,6 @@
     <t>VIRT</t>
   </si>
   <si>
-    <t>Assessing the relation of dual gaze, tutor log, audio and dialog data to students‚Äô learning gains, authors found that a combination of modalities, especially those at a smaller time scale, such as gaze and audio, provides a more accurate prediction of learning gains than models with a single modality.
-Predicting the learning gains via classification (bad, ok, good) through gaze, logs, audio, and dialog. Determined that distance measures between hands and gaze fixations was the key features to predict students' performance.</t>
-  </si>
-  <si>
     <t>embodied conversational agents for multimodal automated social skills training in people with autism spectrum disorders</t>
   </si>
   <si>
@@ -250,10 +246,6 @@
   </si>
   <si>
     <t>ICMI</t>
-  </si>
-  <si>
-    <t>"We observed that linguistic features (i.e.n-gram of various size and types in combination with syntactic information), multimodal in-domain corpora and classification procedures resulted in the best performance on an argument structure mining task."
-"We observed that linguistic features (i.e.n-gram of various size and types in combination with syntactic information), multimodal in-domain corpora and classification procedures resulted in the best performance on an argument structure mining task. Results of the argument quality experiments showed that argument com- prehensibility is affected by the number of referring expressions, information complexity, and presentation fluency. Presence of intensification and segmentation markers, position and movements of hands/ams and certain postures may affect the perception of the clarity, persuasiveness, and credibility of debaters."</t>
   </si>
   <si>
     <t>supervised machine learning in multimodal learning analytics for estimating success in project-based learning</t>
@@ -398,10 +390,6 @@
     <t>MB, MF</t>
   </si>
   <si>
-    <t>We presented two empirical studies, collected in classroom studies with two distinct learning technology systems in different contexts (individual and collaborative). Our analyses and findings showcase a few different ways, in which multimodal data sources can enrich our understanding of student learning and provide a more holistic picture.
-Authors collected student‚Äêfocused screen and webcam video which were useful for understanding students' learning processes and approaches based on detailed analyses of their interactions with the tutor interface, mouse movements, and out‚Äêof‚Äêtutor (in person) help‚Äêseeking. High‚Äêfidelity audio of students' collaborative dialogue was collected to generate high‚Äêquality transcriptions of students' dialogue and apply an NLP approach to make use of the large quantity of audio dialogue. The verbal data allowed authors to identify linguistic features in students' collaborative dialogue that were highly predictive of math performance on pretest and posttest assessments, above and beyond any nonlinguistic variables.</t>
-  </si>
-  <si>
     <t>exploring collaborative writing of user stories with multimodal learning analytics: a case study on a software engineering course</t>
   </si>
   <si>
@@ -519,10 +507,6 @@
   </si>
   <si>
     <t>MLPALA</t>
-  </si>
-  <si>
-    <t>The MMLA techniques applied were able to successfully extract relevant features to quantify and visualize teacher and student behaviors and activities related to student engagement based on the classroom video and audio recordings
-Within heavily rigged smart classroom, visual (gaze, posture) and auditory (speech levels) were extracted via AI and were then used (rule's based approach -&gt; model) to compute student's engagement in individual, pair, and group structures.</t>
   </si>
   <si>
     <t>artificial intelligence and multimodal data in the service of human decision-making: a case study in debate tutoring</t>
@@ -645,12 +629,6 @@
     <t>STATS,PATT</t>
   </si>
   <si>
-    <t>We found that idling with limited speech (i.e., silence or backchannel feedback only) and without movement was negatively correlated with task performance and with participants‚Äô subjective perceptions of the collaboration. However, being silent and focused during solution execution was positively correlated with task performance. Results illustrate that in some cases, multimodal patterns improved the predictions and improved explanatory power over the unimodal primitives.
-"Here, we examine unimodal primitives (activity on the screen, speech, and body movements), and their multimodal combinations during remote CPS."
-Mixed findings for uni- versus multi-modal:
-"These results lead us to question: are the multimodal patterns better than the unimodal primitives? As illustrated above, we found evidence for both sides of the argument. In the case of code execution, the answer is no, but it is a yes in the case of idling. However, it is important to go beyond the significant correlations as there is an informative signal in the non-significant ones as well. For example, consider idling once again. By itself, this pattern is negatively correlated with the task score (r = -.21) and the correlation is even more negative when idling is accompanied by silence/back channeling and little movement (r = -.35). However, there are many other configurations where idling is weak or negligible predictor of task score. For example, idling occurring in the context of the contributors speaking with some movement is more weakly correlated with task score (r = -.11) and the correlation is essentially null when idling is accompanied with the controller speaking and some movement (r = -.06). Thus, even when they do not improve predictive power, multimodal patterns help contextualize and reveal nuances in the unimodal primitives. This supports the overall idea of multimodal learning analytics in which the additional modalities (speech and body movement in our case) help to understand unclear patterns such as idling. This finding is interesting from two perspectives."</t>
-  </si>
-  <si>
     <t>temporal analysis of multimodal data to predict collaborative learning outcomes</t>
   </si>
   <si>
@@ -661,10 +639,6 @@
   </si>
   <si>
     <t>GAZE,LOGS,PROS,TRANS,QUAL</t>
-  </si>
-  <si>
-    <t>Assessing the relation of dual gaze, tutor log, audio and dialog data to students‚Äô learning gains, we find that a combination of modalities, especially those at a smaller time scale, such as gaze and audio, provides a more accurate prediction of learning gains than models with a single modality.
-Evaluating how multimodal features contribute to a model's performance to predict learning gains. Audio features introduce noise that negatively impacted the error of the model.</t>
   </si>
   <si>
     <t>an evaluation of an adaptive learning system based on multimodal affect recognition for learners with intellectual disabilities</t>
@@ -795,10 +769,6 @@
   </si>
   <si>
     <t>MMLA Handbook</t>
-  </si>
-  <si>
-    <t>Results demonstrate how NLP and ML techniques allow us to use different modalities of the same data, voice and transcript, and different modalities of different data sources, voice data from interviews, answers to a goal orientation questionnaire, and answers to open-ended questions about energy, in order to better understand individual differences in students‚Äô performances
-Used text and audio to predict student's affect. With the affect, the authors' explored its statistical relation to student's knowledge. Results point that they need more data to improve performance in affect prediction but promising direction.</t>
   </si>
   <si>
     <t>visualizing collaboration in teamwork: a multimodal learning analytics platform for non-verbal communication</t>
@@ -892,16 +862,6 @@
   </si>
   <si>
     <t>Virtual debate coach.</t>
-  </si>
-  <si>
-    <t>A fully automatic system that is able to understand natu-
-ral arguments in a debate accurately enough to achieve human-like
-performance has not been yet achieved due to certain limitations in
-sensor tracking, speech recognition, and natural language process-
-ing technologies. Also since a data-oriented approach for modelling
-of many debate phenomena has been deployed, the currently avail-
-able quantity and quality of multimodal data are insufficient fortraining statistical machine learning algorithms.
-Hardware issues, data issues.</t>
   </si>
   <si>
     <t>Collaboration, CSCL</t>
@@ -934,7 +894,675 @@
 Complexity</t>
   </si>
   <si>
-    <t>In practice, however, the increased complexity of data resulting from
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Regression:
+Linear Regression (LR), Bayesian, Ridge Regression (BRR) and Support Vector Machine Regression (SVR).</t>
+  </si>
+  <si>
+    <t>Classification:
+Naive Bayesian (NB), Logistic Regression (LR) and Support Vector Machines with linear (SVML) and Gaussian kernel (SVMR).</t>
+  </si>
+  <si>
+    <t>regression: Multiple linear regression for score prediction (0-100) and statistical methods 
+stats: Pre/post test scores t-test to measure effect of the training.</t>
+  </si>
+  <si>
+    <t>qual: descriptive statistics
+clust: k-means
+stats: identify correlations between the multimodal data, experimental condition, and two learning outcomes: design quality and learning.
+Patt: behavior patterns</t>
+  </si>
+  <si>
+    <t>CLS: SVM comparing multimodal to unimodal
+STATS: correlations between individual features and confidence level
+QUAL: descriptive statistics</t>
+  </si>
+  <si>
+    <t>"In line with previous empirical findings, we acknowledge that persuasive speech is rather difficult to characterize."</t>
+  </si>
+  <si>
+    <t>QUAL: descriptive statistics
+STATS: correlations between features and likert scores
+CLS: Support Vector Machine [6], Logistic Regression [75], AdaBoost [76] and the Linear Support Vector Classifier (LinearSVC), Gradient Boosting</t>
+  </si>
+  <si>
+    <t>REG: DNN regression for scoring outcome
+CLS: Naive Bayesian (NB), Logistic Regression (LR) and Support Vector Machines with linear (SVML) and Gaussian kernel (SVMR) (all for outcome classification)</t>
+  </si>
+  <si>
+    <t>Stats: correlate features with collaboration quality, pretest/posttest/gains between two interventions, self-reported vs. researcher-reported collab</t>
+  </si>
+  <si>
+    <t>stats: statistical significance for learning gains
+qual: descriptive statistics, observation, indiviual examples</t>
+  </si>
+  <si>
+    <t>net: Orchestration Graph Extraction
+cls: SVM, RNN
+stats: feature correlation
+patt: markov chains</t>
+  </si>
+  <si>
+    <t>stat: behavior correlation with learning gains
+reg: Additive Factors Model for LR to identify learning trajectories and concentration, linear regression for predicting scores on post-test items related to the balanced reactions knowledge
+qual: observation (watching videos to identify mistakes)</t>
+  </si>
+  <si>
+    <t>cls: additive factors logistic regression model to see if multimodal data improves model performance relative to just using logs
+stats: paired samples t test between students' pretest and posttest scores to assess evidence of learning from the collaborative fraction tutor, linear mixed effects (LMEs) model, p-values</t>
+  </si>
+  <si>
+    <t>Collaborative, Exploring Collaborative Writing of User Stories w/ MMLA</t>
+  </si>
+  <si>
+    <t>Stats: feature correlation
+network: social network analysis
+qual: descriptive statistics</t>
+  </si>
+  <si>
+    <t>RAP system for auto feedback for oral presentation skills. The report starts with an automatically generated summary of
+the overall quality of the presentation. A global score is provided, by
+averaging all the individual scores of each modality. The full video
+of the presentation can be seen in this section. This introduction also
+contains pre-generated advice to improve the perceived weaknesses.</t>
+  </si>
+  <si>
+    <t>Lots of FN for "filled pauses", i.e., low recall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clas: specific method not mentioned, but 2- and 3-way classification
+qual: individual examples via questionnaire </t>
+  </si>
+  <si>
+    <t>collab, agile dev practices</t>
+  </si>
+  <si>
+    <t>net: communication network graph, i.e., who speaks to who
+stats: correlation</t>
+  </si>
+  <si>
+    <t>qual: traditional qualitative methods involving multiple coders
+following a constructivist dialogue mapping approach [9] a type of concept mapping
+[15] on transcripts of interviews and gameplay conversation.</t>
+  </si>
+  <si>
+    <t>Emotion Tracking and Learning
+in Museum Games
+Multiperson but necessarily collaborative</t>
+  </si>
+  <si>
+    <t>Collab. Multimodal techniques to analyze
+the learning activities in a laboratory classroom.</t>
+  </si>
+  <si>
+    <t>Codesign, explainability, trust (challenge/gap as a whole for the field).</t>
+  </si>
+  <si>
+    <t>Generinc CLS/CLUST w/out specific details</t>
+  </si>
+  <si>
+    <t>Debate tutoring case study. Rd</t>
+  </si>
+  <si>
+    <t>CLS: multinomial logistic regression to classify the scores of the candidates.</t>
+  </si>
+  <si>
+    <t>Collaborative. Article explores what multimodal data can tell us about SRL
+processes in collaborative learning tasks, discussing and demonstrating
+how multimodal data can be used for collecting and triangulating data
+about the regulation of learning.</t>
+  </si>
+  <si>
+    <t>QUAL: temporal descriptive statistics based on observation</t>
+  </si>
+  <si>
+    <t>collaborative multimodal composing</t>
+  </si>
+  <si>
+    <t>QUAL: constant comparative method to establish codes
+for types of interactions and the mediating modes as a case study small
+group collaboratively composed.</t>
+  </si>
+  <si>
+    <t>Investigate impact of real-time multimodal student engagement analytics tool in classrooms</t>
+  </si>
+  <si>
+    <t>Overall challenge: class size and data. Majority of methods used to analyze case studies or classroom-sized study participants. This is not a lot of data and may help explain why DL methods are not as common as you would expect.</t>
+  </si>
+  <si>
+    <t>QUAL: interviews, individual quotes
+Stats: significance testing for differences of
+scaffolding interventions
+CLS: specific type not mentioned</t>
+  </si>
+  <si>
+    <t>introduce the concept of
+collaboration translucence, an approach to make visible
+selected features of group activity to give meaning to multimodal data.</t>
+  </si>
+  <si>
+    <t>Explainability: making sense of the data (overall challenge)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUAL: grounding quantitative data in the semantics
+derived from a qualitative interpretation of the context
+from which it arises, qualitative observation of videos for coding, </t>
+  </si>
+  <si>
+    <t>CPS. Multimodal patterns for minecraft. Sometimes unimodal better, sometimes multimodal better.</t>
+  </si>
+  <si>
+    <t>STATS: look at both unimodal and multimodal feature combinations and their correlations with task scores. 
+PATT: behavioral pattern ID</t>
+  </si>
+  <si>
+    <t>small set of students (overall challenge)</t>
+  </si>
+  <si>
+    <t>Collaborative. Temporal analysis of multimodal data to predict collaborative
+learning outcomes. The dyads engaged in an equivalent fractions problem-solving activity using a networked collaborative ITS.</t>
+  </si>
+  <si>
+    <t>REG: LSTM to predict (regress) learning gains</t>
+  </si>
+  <si>
+    <t>Focus on learners with intellectual disabilities. used multimodal sensor data and machine learning to first identify three affective states linked to learning (engagement, frustration, boredom) and second determine the presentation of learning content so that the learner is maintained in an optimal affective state and rate of learning is maximised.</t>
+  </si>
+  <si>
+    <t>limited amount of data available to properly train</t>
+  </si>
+  <si>
+    <t>CLS: CNN, SVM, Linear mixed and log-linear mixed models, multilevel
+mixed effects tobit model
+STATS: Wald z tests were performed under the central limit theorem to test the individual significance of fixed effect coefficients, statistical significance</t>
+  </si>
+  <si>
+    <t>RAP system evaluation.</t>
+  </si>
+  <si>
+    <t>STATS: statistical significance for differences in scores</t>
+  </si>
+  <si>
+    <t>One-on-one coaching. Affect, Support, and Personal Factors:
+Multimodal Causal Models of One-on-one
+Coaching. explore an analytical framework that is explainable and amenable
+to incorporating domain knowledge.</t>
+  </si>
+  <si>
+    <t>the uncertainty arising from the [subjective] annotations may influence the resulting model structures, parameters and interpretation. I.e., tough to generalize (overall challenge)
+the size of the dataset used is relatively small, and the subject pool is not overly diverse, limiting our ability to explore culture or ethics-related factors in the model reliably (oveall challenges)</t>
+  </si>
+  <si>
+    <t>STATS: groups of variables are used as inputs to the Sparse Multiple CCA procedure (Witten and Tibshirani, 2009) to learn a sparse representation for each group by simultaneously maximizing the correlations among the groups of multiple features.
+NET: causal graph search and model estimations.</t>
+  </si>
+  <si>
+    <t>QUAL: The surveys from students were also looked at qualitatively to get
+a general picture of student perceptions. Also used fieldnotes.</t>
+  </si>
+  <si>
+    <t>Multicraft: A Multimodal Interface for Supporting and Studying Learning in Minecraft. First round DBR getting student feedback.</t>
+  </si>
+  <si>
+    <t>Text-input difficult for younger students who couldn't yet type.
+Unreliable ASR. We believe that this is due to poor quality acoustic models for adolescents and because many of our participants spoke other languages at home.</t>
+  </si>
+  <si>
+    <t>MMLA to Explore Collaboration in a Sustainability Co-located Tabletop Game. leveraging MMLA to explore collaboration indicators in a multiplayer, co-located SG for education in sustainable development.</t>
+  </si>
+  <si>
+    <t>STATS: Variables originating from the different sources were examined with descriptive statistics. Perceived quality of
+collaboration was correlated with other variables using Pearson correlations. Teams were then categorised
+according to turn score quartiles, which was then used to analyse the relationship between game performance
+and collaboration behaviours using one-way ANOVA.</t>
+  </si>
+  <si>
+    <t>Collaborative. identifying multi-modal
+behavioral profles of collaborative learning in constructivist
+activities. we describe a combined multi-modal learning analytics and interaction analysis method that uses video, audio and log data to identify multi-modal
+collaborative learning behavioral profles of 32 dyads as they work on an open-ended
+task around interactive tabletops with a robot mediator.</t>
+  </si>
+  <si>
+    <t>"Our combined multi-modal learning analytics and interaction analysis methodology enabled us to identify two multi-modal profles of learners who have learning gains and one multi-modal profle of learners who do not have learning gains."
+"Using this approach, we are able to build the multimodal behavioral profles for each group of learners."
+"Our combined multi-modal learning analytics and interaction analysis methodology enabled us to identify two multi-modal profles of learners who have learning gains and one multi-modal profle of learners who do not have learning gains."
+These profles, which we name Expressive Explorers, Calm Tinkerers, and Silent Wanderers, confrm previous collaborative learning fndings. In particular, the amount of speech interaction and the overlap of speech between a pair of learners are behavior patterns that strongly distinguish between learning and non-learning pairs.</t>
+  </si>
+  <si>
+    <t>STATS: p-values for the Kruskal-Wallis analysis on each pair with signifcance level of 0.05
+QUAL: interaction analysis
+CLUST: cluster learning and performance measures and also multi-modal behaviors
+CLS: SVM and Random Forests</t>
+  </si>
+  <si>
+    <t>The data
+driven clusters are imbalanced, meaning that with our pipeline, the non-learning cluster
+that emerges has fewer teams. This may be one of the reasons why the gainer profles
+are clearer compared to the Silent Wanderers profle (overall challenge)</t>
+  </si>
+  <si>
+    <t>Emotions in MMLA. We use NLP and machine learning
+techniques to automatically extract information about students’ motivational states while engaging in the construction of explanations and investigate how this informa-
+tion can help more accurately predict students’ learning over the course of a 10-week energy unit.</t>
+  </si>
+  <si>
+    <t>CLS: OpenVokaturi SDK emotion detection
+REG: Regression results for valence/discrete emotions. Dependent variable students’ knowledge-in-use about
+energy after the unit. we used regression models to further investigate how valence could help us
+to better understand students’ performance on the energy test after the unit.
+STATS: correlations between valence, students’
+energy knowledge-in-use after the unit, and their mastery goal orientation, w/ p-value</t>
+  </si>
+  <si>
+    <t>Collab. We present a MMLA platform to support
+collaboration assessment based on the capture and classification of non-verbal communication in-
+teractions.</t>
+  </si>
+  <si>
+    <t>QUAL: Case study. we decided to compare two different teamwork activities, with
+high contrast between collaborative and non-collaborative work. Field notes allowed us to describe the flow of interaction of
+the subjects and observations about the six collaboration constructs of the framework</t>
+  </si>
+  <si>
+    <t>Finally, the design and sample size of the focus group do not allow us to generalize the
+results. (overall challenge)</t>
+  </si>
+  <si>
+    <t>Recurrence Quantification Analysis (RQA) to quantify the
+microgenesis of stable new patterns in hand movement and gaze.</t>
+  </si>
+  <si>
+    <t>PATT: Recurrence Quantification Analysis (RQA)
+QUAL: To contextualize results within the student’s
+specific learning trajectory, we began with a qualitative analysis of the audio-video
+recording.
+STATS: We also calculated the correlation between each hand’s y-location and
+y-axis gaze position in each task stage as an initial reflection of the relationship
+between these two modalities.</t>
+  </si>
+  <si>
+    <t>Collab. A multimodal analysis of pair work engagement episodes:
+Implications for EMI lecturer training.</t>
+  </si>
+  <si>
+    <t>QUAL: In the first part, the 12 micro-teaching sessions were carefully watched to identify the pair work EEs (See Table 1). Then, the
+selected EEs were transcribed and examined to determine the moves and pedagogical functions the lecturers performed. In the second part, the microanalysis, we followed a SF-MDA (O’Halloran, 2004) approach to describe how these pedagogical
+functions were constructed multimodally.</t>
+  </si>
+  <si>
+    <t>Collab. This paper inves-
+tigates multimodal detection of impasse by analyzing 46 middle
+school learners’ collaborative dialogue—including speech and facial
+behaviors—during a coding task.</t>
+  </si>
+  <si>
+    <t>CLS: (Speaker-aware) Fine-tuned BERT for impasse classification (and regular fine-tuned BERT), TF-IDF, Word2Vec. Also used SVM, MLP to identify predictive unimodal features.</t>
+  </si>
+  <si>
+    <t>our corpus size was relatively small.
+The recordings were collected from just 46 middle school learners; (overall challenge)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We presented two empirical studies, collected in classroom studies with two distinct learning technology systems in different contexts (individual and collaborative). Our analyses and findings showcase a few different ways, in which multimodal data sources can enrich our understanding of student learning and provide a more holistic picture.
+Authors collected student‚Äêfocused screen and webcam video which were useful for understanding students' learning processes and approaches based on detailed analyses of their interactions with the tutor interface, mouse movements, and out‚Äêof‚Äêtutor (in person) help‚Äêseeking. High‚Äêfidelity audio of students' collaborative dialogue was collected to generate high‚Äêquality transcriptions of students' dialogue and apply an NLP approach to make use of the large quantity of audio dialogue. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The verbal data allowed authors to identify linguistic features in students' collaborative dialogue that were highly predictive of math performance on pretest and posttest assessments, above and beyond any nonlinguistic variables.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"We observed that linguistic features (i.e.n-gram of various size and types in combination with syntactic information), multimodal in-domain corpora and classification procedures resulted in the best performance on an argument structure mining task."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"We observed that linguistic features (i.e.n-gram of various size and types in combination with syntactic information), multimodal in-domain corpora and classification procedures resulted in the best performance on an argument structure mining task. Results of the argument quality experiments showed that argument com- prehensibility is affected by the number of referring expressions, information complexity, and presentation fluency. Presence of intensification and segmentation markers, position and movements of hands/ams and certain postures may affect the perception of the clarity, persuasiveness, and credibility of debaters."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The MMLA techniques applied were able to successfully extract relevant features to quantify and visualize teacher and student behaviors and activities related to student engagement based on the classroom video and audio recordings
+Within heavily rigged smart classroom, visual (gaze, posture) and auditory (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>speech levels</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) were extracted via AI and were then used (rule's based approach -&gt; model) to compute student's engagement in individual, pair, and group structures.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We found that idling with limited speech (i.e., silence or backchannel feedback only) and without movement was negatively correlated with task performance and with participants‚Äô subjective perceptions of the collaboration. However, being silent and focused during solution execution was positively correlated with task performance. Results illustrate that in some cases, multimodal patterns improved the predictions and improved explanatory power over the unimodal primitives.
+"Here, we examine unimodal primitives (activity on the screen, speech, and body movements), and their multimodal combinations during remote CPS."
+Mixed findings for uni- versus multi-modal:
+"These results lead us to question: are the multimodal patterns better than the unimodal primitives? As illustrated above, we found evidence for both sides of the argument. In the case of code execution, the answer is no, but it is a yes in the case of idling. However, it is important to go beyond the significant correlations as there is an informative signal in the non-significant ones as well. For example, consider idling once again. By itself, this pattern is negatively correlated with the task score (r = -.21) and the correlation is even more negative when idling is accompanied by silence/back channeling and little movement (r = -.35). However, there are many other configurations where idling is weak or negligible predictor of task score. For example, idling occurring in the context of the contributors speaking with some movement is more weakly correlated with task score (r = -.11) and the correlation is essentially null when idling is accompanied with the controller speaking and some movement (r = -.06). </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Thus, even when they do not improve predictive power, multimodal patterns help contextualize and reveal nuances in the unimodal primitives.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This supports the overall idea of multimodal learning analytics in which the additional modalities (speech and body movement in our case) help to understand unclear patterns such as idling.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This finding is interesting from two perspectives."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Assessing the relation of dual gaze, tutor log, audio and dialog data to students‚Äô learning gains, we find that a combination of modalities, especially those at a smaller time scale, such as gaze and audio, provides a more accurate prediction of learning gains than models with a single modality.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Evaluating how multimodal features contribute to a model's performance to predict learning gains. Audio features introduce noise that negatively impacted the error of the model.</t>
+    </r>
+  </si>
+  <si>
+    <t>Predicting the learning gains via classification (bad, ok, good) through gaze, logs, audio, and dialog. Determined that distance measures between hands and gaze fixations was the key features to predict students' performance.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Results demonstrate how NLP and ML techniques allow us to use different modalities of the same data, voice and transcript, and different modalities of different data sources, voice data from interviews, answers to a goal orientation questionnaire, and answers to open-ended questions about energy, in order to better understand individual differences in students‚Äô performances</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Used text and audio to predict student's affect. With the affect, the authors' explored its statistical relation to student's knowledge. Results point that they need more data to improve performance in affect prediction but promising direction.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"We found that the semantics and speaker information in the linguistic modality, the pitch variation in the audio modality, and the facial muscle movements in the video modality are the most significant unimodal indicators of impasse."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"We found that the semantics and speaker information in the linguistic modality, the pitch variation in the audio modality, and the facial muscle movements in the video modality are the most significant unimodal indicators of impasse. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>We also trained several multimodal models and found that combining indicators from these three modalities provided the best impasse detection performance."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The results showed that Linguistic + Audio + Video (F1 Score
+= 0.65) yielded the best impasse detection performance, and Audio
++ Video (F1 Score = 0.39) performed the worst. There are several
+important implications behind these results. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>First, all of our multi-
+modal models outperformed their unimodal models (e.g., the Audio
++ Video model outperformed unimodal Audio / Video models, the
+Linguistic + Audio model outperformed unimodal Linguistic / Au-
+dio models), which indicated that combining modalities improves
+impasse detection performance. Second, the close performance from
+the Linguistic + Video model and the Linguistic + Audio + Video
+model suggested that adding acoustic-prosodic features to the Lin-
+guistic + Video model did not make a substantial difference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. As
+we discussed in section 6.1.2, the significant rise in pitch when the
+second learner started talking was more correlated with impasse
+moments when learners expressed disagreement;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A fully automatic system that is able to understand natu-
+ral arguments in a debate accurately enough to achieve human-like
+performance has not been yet achieved due to certain limitations in
+sensor tracking, speech recognition, and natural language process-
+ing technologies. Also since a data-oriented approach for modelling
+of many debate phenomena has been deployed, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the currently avail-
+able quantity and quality of multimodal data are insufficient fortraining statistical machine learning algorithms.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Hardware issues, data issues.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>for complexity challenge: "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The eye-tracking glasses sampled at a rate of 50
+Hz, thus generating roughly 90,000 data points per person during the 30-minute session.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" (Overall challenge)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Indeed, the understanding of specific problems and phenomena that arise in the implementation of educational innovations in authentic settings (also known as ‘orchestration’) is considered one of the foremost challenges in the
+field of TEL (Fischer et al. 2014; Roschelle et al. 2013).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>From the audio data, 6405 features were extracted</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> using the openSMILE audio
+processing toolkit (http://audeering.com/technology/opensmile/). The features
+extracted included both high-level constructs (e.g., emotion detection
+predictions) as well as low-level features of the spectrum, energy, etc. of each
+episode (commonly used in audio data mining and machine learning challenges).
+Complexity with so many features.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In practice, however, the increased complexity of data resulting from
 adding new, multimodal data streams from different sources can create
 many challenges. These data are often collected at different grain sizes,
 which are difficult to integrate. Making sense of data at many levels of
@@ -943,288 +1571,62 @@
 exhibits as he or she engages in productive struggle with a difficult
 concept and the social interactions surrounding this struggle. To fully
 understand the events that unfold even in this small segment of a
-student's educational experience, a researcher may need to watch screen
+student's educational experience, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a researcher may need to watch screen
 video data, listen to the audio dialogue several times, and enter
 behavioural codes into a separate document. Having to do this for every
 problem and concept students experience over the course of even one
 class period of learning technology use would be vastly taxing on human
-time and effort. Yet this level of detailed analysis provides interesting and
+time and effort.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Yet this level of detailed analysis provides interesting and
 temporally rich insights (Worsley, 2014), in contrast to purely quantitative
 models based solely on coarse‐level “correctness” coding.
-One of the biggest challenges in multimodal learning analytics is
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">One of the biggest challenges in multimodal learning analytics is
 that the large volume of rich, multimodal data collected requires signif-
 icant human time and effort to make sense of.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Complexity</t>
-  </si>
-  <si>
-    <t>for complexity challenge: "The eye-tracking glasses sampled at a rate of 50
-Hz, thus generating roughly 90,000 data points per person during the 30-minute session."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indeed, the understanding of specific problems and phenomena that arise in the implementation of educational innovations in authentic settings (also known as ‘orchestration’) is considered one of the foremost challenges in the
-field of TEL (Fischer et al. 2014; Roschelle et al. 2013).
-From the audio data, 6405 features were extracted using the openSMILE audio
-processing toolkit (http://audeering.com/technology/opensmile/). The features
-extracted included both high-level constructs (e.g., emotion detection
-predictions) as well as low-level features of the spectrum, energy, etc. of each
-episode (commonly used in audio data mining and machine learning challenges).
-Complexity with so many features.
-</t>
-  </si>
-  <si>
-    <t>Analysis</t>
-  </si>
-  <si>
-    <t>Regression:
-Linear Regression (LR), Bayesian, Ridge Regression (BRR) and Support Vector Machine Regression (SVR).</t>
-  </si>
-  <si>
-    <t>Classification:
-Naive Bayesian (NB), Logistic Regression (LR) and Support Vector Machines with linear (SVML) and Gaussian kernel (SVMR).</t>
-  </si>
-  <si>
-    <t>regression: Multiple linear regression for score prediction (0-100) and statistical methods 
-stats: Pre/post test scores t-test to measure effect of the training.</t>
-  </si>
-  <si>
-    <t>qual: descriptive statistics
-clust: k-means
-stats: identify correlations between the multimodal data, experimental condition, and two learning outcomes: design quality and learning.
-Patt: behavior patterns</t>
-  </si>
-  <si>
-    <t>CLS: SVM comparing multimodal to unimodal
-STATS: correlations between individual features and confidence level
-QUAL: descriptive statistics</t>
-  </si>
-  <si>
-    <t>"In line with previous empirical findings, we acknowledge that persuasive speech is rather difficult to characterize."</t>
-  </si>
-  <si>
-    <t>QUAL: descriptive statistics
-STATS: correlations between features and likert scores
-CLS: Support Vector Machine [6], Logistic Regression [75], AdaBoost [76] and the Linear Support Vector Classifier (LinearSVC), Gradient Boosting</t>
-  </si>
-  <si>
-    <t>REG: DNN regression for scoring outcome
-CLS: Naive Bayesian (NB), Logistic Regression (LR) and Support Vector Machines with linear (SVML) and Gaussian kernel (SVMR) (all for outcome classification)</t>
-  </si>
-  <si>
-    <t>Stats: correlate features with collaboration quality, pretest/posttest/gains between two interventions, self-reported vs. researcher-reported collab</t>
-  </si>
-  <si>
-    <t>stats: statistical significance for learning gains
-qual: descriptive statistics, observation, indiviual examples</t>
-  </si>
-  <si>
-    <t>net: Orchestration Graph Extraction
-cls: SVM, RNN
-stats: feature correlation
-patt: markov chains</t>
-  </si>
-  <si>
-    <t>stat: behavior correlation with learning gains
-reg: Additive Factors Model for LR to identify learning trajectories and concentration, linear regression for predicting scores on post-test items related to the balanced reactions knowledge
-qual: observation (watching videos to identify mistakes)</t>
-  </si>
-  <si>
-    <t>cls: additive factors logistic regression model to see if multimodal data improves model performance relative to just using logs
-stats: paired samples t test between students' pretest and posttest scores to assess evidence of learning from the collaborative fraction tutor, linear mixed effects (LMEs) model, p-values</t>
-  </si>
-  <si>
-    <t>Collaborative, Exploring Collaborative Writing of User Stories w/ MMLA</t>
-  </si>
-  <si>
-    <t>Stats: feature correlation
-network: social network analysis
-qual: descriptive statistics</t>
-  </si>
-  <si>
-    <t>RAP system for auto feedback for oral presentation skills. The report starts with an automatically generated summary of
-the overall quality of the presentation. A global score is provided, by
-averaging all the individual scores of each modality. The full video
-of the presentation can be seen in this section. This introduction also
-contains pre-generated advice to improve the perceived weaknesses.</t>
-  </si>
-  <si>
-    <t>Lots of FN for "filled pauses", i.e., low recall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clas: specific method not mentioned, but 2- and 3-way classification
-qual: individual examples via questionnaire </t>
-  </si>
-  <si>
-    <t>collab, agile dev practices</t>
-  </si>
-  <si>
-    <t>net: communication network graph, i.e., who speaks to who
-stats: correlation</t>
-  </si>
-  <si>
-    <t>qual: traditional qualitative methods involving multiple coders
-following a constructivist dialogue mapping approach [9] a type of concept mapping
-[15] on transcripts of interviews and gameplay conversation.</t>
-  </si>
-  <si>
-    <t>Emotion Tracking and Learning
-in Museum Games
-Multiperson but necessarily collaborative</t>
-  </si>
-  <si>
-    <t>Collab. Multimodal techniques to analyze
-the learning activities in a laboratory classroom.</t>
-  </si>
-  <si>
-    <t>Codesign, explainability, trust (challenge/gap as a whole for the field).</t>
-  </si>
-  <si>
-    <t>Generinc CLS/CLUST w/out specific details</t>
-  </si>
-  <si>
-    <t>Debate tutoring case study. Rd</t>
-  </si>
-  <si>
-    <t>CLS: multinomial logistic regression to classify the scores of the candidates.</t>
-  </si>
-  <si>
-    <t>Collaborative. Article explores what multimodal data can tell us about SRL
-processes in collaborative learning tasks, discussing and demonstrating
-how multimodal data can be used for collecting and triangulating data
-about the regulation of learning.</t>
-  </si>
-  <si>
-    <t>QUAL: temporal descriptive statistics based on observation</t>
-  </si>
-  <si>
-    <t>collaborative multimodal composing</t>
-  </si>
-  <si>
-    <t>QUAL: constant comparative method to establish codes
-for types of interactions and the mediating modes as a case study small
-group collaboratively composed.</t>
-  </si>
-  <si>
-    <t>Investigate impact of real-time multimodal student engagement analytics tool in classrooms</t>
-  </si>
-  <si>
-    <t>Overall challenge: class size and data. Majority of methods used to analyze case studies or classroom-sized study participants. This is not a lot of data and may help explain why DL methods are not as common as you would expect.</t>
-  </si>
-  <si>
-    <t>QUAL: interviews, individual quotes
-Stats: significance testing for differences of
-scaffolding interventions
-CLS: specific type not mentioned</t>
-  </si>
-  <si>
-    <t>introduce the concept of
-collaboration translucence, an approach to make visible
-selected features of group activity to give meaning to multimodal data.</t>
-  </si>
-  <si>
-    <t>Explainability: making sense of the data (overall challenge)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUAL: grounding quantitative data in the semantics
-derived from a qualitative interpretation of the context
-from which it arises, qualitative observation of videos for coding, </t>
-  </si>
-  <si>
-    <t>CPS. Multimodal patterns for minecraft. Sometimes unimodal better, sometimes multimodal better.</t>
-  </si>
-  <si>
-    <t>STATS: look at both unimodal and multimodal feature combinations and their correlations with task scores. 
-PATT: behavioral pattern ID</t>
-  </si>
-  <si>
-    <t>small set of students (overall challenge)</t>
-  </si>
-  <si>
-    <t>Collaborative. Temporal analysis of multimodal data to predict collaborative
-learning outcomes. The dyads engaged in an equivalent fractions problem-solving activity using a networked collaborative ITS.</t>
-  </si>
-  <si>
-    <t>REG: LSTM to predict (regress) learning gains</t>
-  </si>
-  <si>
-    <t>Focus on learners with intellectual disabilities. used multimodal sensor data and machine learning to first identify three affective states linked to learning (engagement, frustration, boredom) and second determine the presentation of learning content so that the learner is maintained in an optimal affective state and rate of learning is maximised.</t>
-  </si>
-  <si>
-    <t>limited amount of data available to properly train</t>
-  </si>
-  <si>
-    <t>CLS: CNN, SVM, Linear mixed and log-linear mixed models, multilevel
-mixed effects tobit model
-STATS: Wald z tests were performed under the central limit theorem to test the individual significance of fixed effect coefficients, statistical significance</t>
-  </si>
-  <si>
-    <t>RAP system evaluation.</t>
-  </si>
-  <si>
-    <t>STATS: statistical significance for differences in scores</t>
-  </si>
-  <si>
-    <t>One-on-one coaching. Affect, Support, and Personal Factors:
-Multimodal Causal Models of One-on-one
-Coaching. explore an analytical framework that is explainable and amenable
-to incorporating domain knowledge.</t>
-  </si>
-  <si>
-    <t>the uncertainty arising from the [subjective] annotations may influence the resulting model structures, parameters and interpretation. I.e., tough to generalize (overall challenge)
-the size of the dataset used is relatively small, and the subject pool is not overly diverse, limiting our ability to explore culture or ethics-related factors in the model reliably (oveall challenges)</t>
-  </si>
-  <si>
-    <t>STATS: groups of variables are used as inputs to the Sparse Multiple CCA procedure (Witten and Tibshirani, 2009) to learn a sparse representation for each group by simultaneously maximizing the correlations among the groups of multiple features.
-NET: causal graph search and model estimations.</t>
-  </si>
-  <si>
-    <t>QUAL: The surveys from students were also looked at qualitatively to get
-a general picture of student perceptions. Also used fieldnotes.</t>
-  </si>
-  <si>
-    <t>Multicraft: A Multimodal Interface for Supporting and Studying Learning in Minecraft. First round DBR getting student feedback.</t>
-  </si>
-  <si>
-    <t>Text-input difficult for younger students who couldn't yet type.
-Unreliable ASR. We believe that this is due to poor quality acoustic models for adolescents and because many of our participants spoke other languages at home.</t>
-  </si>
-  <si>
-    <t>MMLA to Explore Collaboration in a Sustainability Co-located Tabletop Game. leveraging MMLA to explore collaboration indicators in a multiplayer, co-located SG for education in sustainable development.</t>
-  </si>
-  <si>
-    <t>STATS: Variables originating from the different sources were examined with descriptive statistics. Perceived quality of
-collaboration was correlated with other variables using Pearson correlations. Teams were then categorised
-according to turn score quartiles, which was then used to analyse the relationship between game performance
-and collaboration behaviours using one-way ANOVA.</t>
-  </si>
-  <si>
-    <t>Collaborative. identifying multi-modal
-behavioral profles of collaborative learning in constructivist
-activities. we describe a combined multi-modal learning analytics and interaction analysis method that uses video, audio and log data to identify multi-modal
-collaborative learning behavioral profles of 32 dyads as they work on an open-ended
-task around interactive tabletops with a robot mediator.</t>
-  </si>
-  <si>
-    <t>"Our combined multi-modal learning analytics and interaction analysis methodology enabled us to identify two multi-modal profles of learners who have learning gains and one multi-modal profle of learners who do not have learning gains."
-"Using this approach, we are able to build the multimodal behavioral profles for each group of learners."
-"Our combined multi-modal learning analytics and interaction analysis methodology enabled us to identify two multi-modal profles of learners who have learning gains and one multi-modal profle of learners who do not have learning gains."
-These profles, which we name Expressive Explorers, Calm Tinkerers, and Silent Wanderers, confrm previous collaborative learning fndings. In particular, the amount of speech interaction and the overlap of speech between a pair of learners are behavior patterns that strongly distinguish between learning and non-learning pairs.</t>
-  </si>
-  <si>
-    <t>STATS: p-values for the Kruskal-Wallis analysis on each pair with signifcance level of 0.05
-QUAL: interaction analysis
-CLUST: cluster learning and performance measures and also multi-modal behaviors
-CLS: SVM and Random Forests</t>
-  </si>
-  <si>
-    <t>The data
-driven clusters are imbalanced, meaning that with our pipeline, the non-learning cluster
-that emerges has fewer teams. This may be one of the reasons why the gainer profles
-are clearer compared to the Silent Wanderers profle (overall challenge)</t>
-  </si>
-  <si>
-    <t>Emotions in MMLA. We use NLP and machine learning
-techniques to automatically extract information about students’ motivational states while engaging in the construction of explanations and investigate how this informa-
-tion can help more accurately predict students’ learning over the course of a 10-week energy unit.</t>
+    </r>
   </si>
   <si>
     <t>extensive preprocessing of the data and the results need to be
@@ -1246,91 +1648,13 @@
 of education (overall challenge)
 data is limited, which represents one of the major
 challenges for building robust and reliable multimodal models. (oveall challenge)
-training a
-model on a reduced dataset introduces a bias to the model, affecting the validity
+training a model on a reduced dataset introduces a bias to the model, affecting the validity
 of the model’s predictions when the data inputs come from a different distribution
 than the training set. (oveall challenge)
 lack of representative data in open datasets (i.e., few focusing on children/education) (overall challenge)</t>
   </si>
   <si>
-    <t>CLS: OpenVokaturi SDK emotion detection
-REG: Regression results for valence/discrete emotions. Dependent variable students’ knowledge-in-use about
-energy after the unit. we used regression models to further investigate how valence could help us
-to better understand students’ performance on the energy test after the unit.
-STATS: correlations between valence, students’
-energy knowledge-in-use after the unit, and their mastery goal orientation, w/ p-value</t>
-  </si>
-  <si>
-    <t>Collab. We present a MMLA platform to support
-collaboration assessment based on the capture and classification of non-verbal communication in-
-teractions.</t>
-  </si>
-  <si>
-    <t>QUAL: Case study. we decided to compare two different teamwork activities, with
-high contrast between collaborative and non-collaborative work. Field notes allowed us to describe the flow of interaction of
-the subjects and observations about the six collaboration constructs of the framework</t>
-  </si>
-  <si>
-    <t>Finally, the design and sample size of the focus group do not allow us to generalize the
-results. (overall challenge)</t>
-  </si>
-  <si>
-    <t>Recurrence Quantification Analysis (RQA) to quantify the
-microgenesis of stable new patterns in hand movement and gaze.</t>
-  </si>
-  <si>
-    <t>PATT: Recurrence Quantification Analysis (RQA)
-QUAL: To contextualize results within the student’s
-specific learning trajectory, we began with a qualitative analysis of the audio-video
-recording.
-STATS: We also calculated the correlation between each hand’s y-location and
-y-axis gaze position in each task stage as an initial reflection of the relationship
-between these two modalities.</t>
-  </si>
-  <si>
-    <t>Collab. A multimodal analysis of pair work engagement episodes:
-Implications for EMI lecturer training.</t>
-  </si>
-  <si>
-    <t>Data scarcity: The limited number of pair work EEs does not allow us to make any strong claims in terms of
-the framework’s reliability. (overall challenge)</t>
-  </si>
-  <si>
-    <t>QUAL: In the first part, the 12 micro-teaching sessions were carefully watched to identify the pair work EEs (See Table 1). Then, the
-selected EEs were transcribed and examined to determine the moves and pedagogical functions the lecturers performed. In the second part, the microanalysis, we followed a SF-MDA (O’Halloran, 2004) approach to describe how these pedagogical
-functions were constructed multimodally.</t>
-  </si>
-  <si>
-    <t>Collab. This paper inves-
-tigates multimodal detection of impasse by analyzing 46 middle
-school learners’ collaborative dialogue—including speech and facial
-behaviors—during a coding task.</t>
-  </si>
-  <si>
-    <t>CLS: (Speaker-aware) Fine-tuned BERT for impasse classification (and regular fine-tuned BERT), TF-IDF, Word2Vec. Also used SVM, MLP to identify predictive unimodal features.</t>
-  </si>
-  <si>
-    <t>our corpus size was relatively small.
-The recordings were collected from just 46 middle school learners; (overall challenge)</t>
-  </si>
-  <si>
-    <t>"We found that the semantics and speaker information in the linguistic modality, the pitch variation in the audio modality, and the facial muscle movements in the video modality are the most significant unimodal indicators of impasse."
-"We found that the semantics and speaker information in the linguistic modality, the pitch variation in the audio modality, and the facial muscle movements in the video modality are the most significant unimodal indicators of impasse. We also trained several multimodal models and found that combining indicators from these three modalities provided the best impasse detection performance."
-The results showed that Linguistic + Audio + Video (F1 Score
-= 0.65) yielded the best impasse detection performance, and Audio
-+ Video (F1 Score = 0.39) performed the worst. There are several
-important implications behind these results. First, all of our multi-
-modal models outperformed their unimodal models (e.g., the Audio
-+ Video model outperformed unimodal Audio / Video models, the
-Linguistic + Audio model outperformed unimodal Linguistic / Au-
-dio models), which indicated that combining modalities improves
-impasse detection performance. Second, the close performance from
-the Linguistic + Video model and the Linguistic + Audio + Video
-model suggested that adding acoustic-prosodic features to the Lin-
-guistic + Video model did not make a substantial difference. As
-we discussed in section 6.1.2, the significant rise in pitch when the
-second learner started talking was more correlated with impasse
-moments when learners expressed disagreement;</t>
+    <t>Data scarcity: The limited number of pair work EEs does not allow us to make any strong claims in terms of the framework’s reliability. (overall challenge)</t>
   </si>
 </sst>
 </file>
@@ -1823,12 +2147,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2189,8 +2519,8 @@
   <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S36" sqref="S36"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="77.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2269,13 +2599,13 @@
         <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="119" x14ac:dyDescent="0.2">
@@ -2331,16 +2661,16 @@
         <v>31</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="136" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>3339002981</v>
       </c>
@@ -2389,14 +2719,14 @@
       <c r="P3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>38</v>
+      <c r="Q3" s="4" t="s">
+        <v>344</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="221" x14ac:dyDescent="0.2">
@@ -2404,58 +2734,58 @@
         <v>3093310941</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D4" s="1">
         <v>2017</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="S4" s="1" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="306" x14ac:dyDescent="0.2">
@@ -2463,10 +2793,10 @@
         <v>3095923626</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D5" s="1">
         <v>2017</v>
@@ -2475,19 +2805,19 @@
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>25</v>
@@ -2499,22 +2829,22 @@
         <v>27</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="204" x14ac:dyDescent="0.2">
@@ -2522,61 +2852,61 @@
         <v>85990093</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D6" s="1">
         <v>2017</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="204" x14ac:dyDescent="0.2">
@@ -2584,61 +2914,61 @@
         <v>957160695</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1">
         <v>2017</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>73</v>
+        <v>340</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>267</v>
+        <v>347</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="356" x14ac:dyDescent="0.2">
@@ -2646,7 +2976,7 @@
         <v>1637690235</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
@@ -2658,22 +2988,22 @@
         <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>26</v>
@@ -2691,13 +3021,13 @@
         <v>30</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
@@ -2705,10 +3035,10 @@
         <v>2181637610</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D9" s="1">
         <v>2018</v>
@@ -2717,22 +3047,22 @@
         <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="K9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>26</v>
@@ -2741,25 +3071,25 @@
         <v>27</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="T9" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="187" x14ac:dyDescent="0.2">
@@ -2767,10 +3097,10 @@
         <v>3146393211</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D10" s="1">
         <v>2018</v>
@@ -2779,28 +3109,28 @@
         <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="K10" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>28</v>
@@ -2809,19 +3139,19 @@
         <v>29</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="221" x14ac:dyDescent="0.2">
@@ -2829,10 +3159,10 @@
         <v>3135645357</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D11" s="1">
         <v>2018</v>
@@ -2841,19 +3171,19 @@
         <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>25</v>
@@ -2868,22 +3198,22 @@
         <v>28</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>277</v>
+        <v>349</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="306" x14ac:dyDescent="0.2">
@@ -2891,10 +3221,10 @@
         <v>3783339081</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D12" s="1">
         <v>2018</v>
@@ -2903,19 +3233,19 @@
         <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>37</v>
@@ -2924,28 +3254,28 @@
         <v>26</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>274</v>
+        <v>108</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="388" x14ac:dyDescent="0.2">
@@ -2953,10 +3283,10 @@
         <v>3796180663</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D13" s="1">
         <v>2018</v>
@@ -2965,19 +3295,19 @@
         <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>37</v>
@@ -2986,28 +3316,28 @@
         <v>26</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>117</v>
+        <v>339</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>275</v>
+        <v>350</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="221" x14ac:dyDescent="0.2">
@@ -3015,10 +3345,10 @@
         <v>2345021698</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D14" s="1">
         <v>2018</v>
@@ -3027,19 +3357,19 @@
         <v>19</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>25</v>
@@ -3051,22 +3381,22 @@
         <v>27</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="238" x14ac:dyDescent="0.2">
@@ -3074,43 +3404,43 @@
         <v>2497456347</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D15" s="1">
         <v>2018</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="K15" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>29</v>
@@ -3119,16 +3449,16 @@
         <v>30</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="170" x14ac:dyDescent="0.2">
@@ -3136,10 +3466,10 @@
         <v>4019205162</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D16" s="1">
         <v>2019</v>
@@ -3148,19 +3478,19 @@
         <v>19</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>25</v>
@@ -3178,16 +3508,16 @@
         <v>29</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="204" x14ac:dyDescent="0.2">
@@ -3195,10 +3525,10 @@
         <v>1847468084</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D17" s="1">
         <v>2019</v>
@@ -3207,19 +3537,19 @@
         <v>19</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>37</v>
@@ -3231,22 +3561,22 @@
         <v>27</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="119" x14ac:dyDescent="0.2">
@@ -3254,10 +3584,10 @@
         <v>1326191931</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D18" s="1">
         <v>2019</v>
@@ -3266,19 +3596,19 @@
         <v>19</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>25</v>
@@ -3287,28 +3617,28 @@
         <v>26</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>154</v>
+        <v>341</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="204" x14ac:dyDescent="0.2">
@@ -3316,10 +3646,10 @@
         <v>1576545447</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D19" s="1">
         <v>2019</v>
@@ -3328,10 +3658,10 @@
         <v>19</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>35</v>
@@ -3340,34 +3670,34 @@
         <v>23</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="L19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="O19" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="289" x14ac:dyDescent="0.2">
@@ -3375,10 +3705,10 @@
         <v>3398902089</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D20" s="1">
         <v>2019</v>
@@ -3387,22 +3717,22 @@
         <v>19</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>26</v>
@@ -3414,19 +3744,19 @@
         <v>28</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
@@ -3434,10 +3764,10 @@
         <v>86191824</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D21" s="1">
         <v>2019</v>
@@ -3446,19 +3776,19 @@
         <v>19</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>37</v>
@@ -3473,19 +3803,19 @@
         <v>28</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="102" x14ac:dyDescent="0.2">
@@ -3493,10 +3823,10 @@
         <v>3448122334</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D22" s="1">
         <v>2019</v>
@@ -3505,19 +3835,19 @@
         <v>19</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>37</v>
@@ -3526,28 +3856,28 @@
         <v>26</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="153" x14ac:dyDescent="0.2">
@@ -3555,31 +3885,31 @@
         <v>1296637108</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D23" s="1">
         <v>2019</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>25</v>
@@ -3591,7 +3921,7 @@
         <v>27</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>29</v>
@@ -3600,16 +3930,16 @@
         <v>30</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
@@ -3617,10 +3947,10 @@
         <v>1770989706</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D24" s="1">
         <v>2020</v>
@@ -3629,19 +3959,19 @@
         <v>19</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>37</v>
@@ -3659,16 +3989,16 @@
         <v>29</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>190</v>
+        <v>342</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="119" x14ac:dyDescent="0.2">
@@ -3676,10 +4006,10 @@
         <v>3051560548</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D25" s="1">
         <v>2020</v>
@@ -3688,10 +4018,10 @@
         <v>19</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>22</v>
@@ -3700,7 +4030,7 @@
         <v>23</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>37</v>
@@ -3715,22 +4045,22 @@
         <v>28</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>195</v>
+        <v>343</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="255" x14ac:dyDescent="0.2">
@@ -3738,10 +4068,10 @@
         <v>3796643912</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D26" s="1">
         <v>2020</v>
@@ -3750,49 +4080,49 @@
         <v>19</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>37</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="136" x14ac:dyDescent="0.2">
@@ -3800,58 +4130,58 @@
         <v>2634033325</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D27" s="1">
         <v>2020</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="O27" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="153" x14ac:dyDescent="0.2">
@@ -3859,10 +4189,10 @@
         <v>1426267857</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D28" s="1">
         <v>2021</v>
@@ -3871,19 +4201,19 @@
         <v>19</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>25</v>
@@ -3892,28 +4222,28 @@
         <v>26</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="221" x14ac:dyDescent="0.2">
@@ -3921,10 +4251,10 @@
         <v>666050348</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="1">
         <v>2021</v>
@@ -3933,19 +4263,19 @@
         <v>19</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>37</v>
@@ -3954,28 +4284,28 @@
         <v>26</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="T29" s="1" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="388" x14ac:dyDescent="0.2">
@@ -3983,10 +4313,10 @@
         <v>518268671</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D30" s="1">
         <v>2021</v>
@@ -3995,22 +4325,22 @@
         <v>19</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>26</v>
@@ -4025,16 +4355,16 @@
         <v>29</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="255" x14ac:dyDescent="0.2">
@@ -4042,10 +4372,10 @@
         <v>2273914836</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D31" s="1">
         <v>2022</v>
@@ -4054,22 +4384,22 @@
         <v>19</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>26</v>
@@ -4081,22 +4411,22 @@
         <v>28</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
@@ -4104,10 +4434,10 @@
         <v>32184286</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D32" s="1">
         <v>2022</v>
@@ -4116,19 +4446,19 @@
         <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>25</v>
@@ -4137,28 +4467,28 @@
         <v>26</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>237</v>
+        <v>345</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="T32" s="1" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="238" x14ac:dyDescent="0.2">
@@ -4166,10 +4496,10 @@
         <v>2609260641</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D33" s="1">
         <v>2022</v>
@@ -4178,49 +4508,49 @@
         <v>19</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="T33" s="1" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="238" x14ac:dyDescent="0.2">
@@ -4228,10 +4558,10 @@
         <v>1345598079</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="D34" s="1">
         <v>2022</v>
@@ -4240,19 +4570,19 @@
         <v>19</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>37</v>
@@ -4261,25 +4591,25 @@
         <v>26</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="187" x14ac:dyDescent="0.2">
@@ -4287,61 +4617,61 @@
         <v>2155422499</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D35" s="1">
         <v>2022</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>27</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
@@ -4349,10 +4679,10 @@
         <v>3754172825</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D36" s="1">
         <v>2022</v>
@@ -4361,19 +4691,19 @@
         <v>19</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>37</v>
@@ -4388,22 +4718,22 @@
         <v>28</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P36" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="T36" s="1" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>